<commit_message>
fix : inconsistent import
</commit_message>
<xml_diff>
--- a/docs/clean.xlsx
+++ b/docs/clean.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d233ac7338db6ff3/Dokumen/Kost Man/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gunaw\KostMan\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{1F7C46C9-7B8B-4CA3-87B3-54B5BAB0FEC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9A4A3789-0DB8-4C03-BD7F-601E166B9DE2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FEA1A6-8FCF-49F8-9C8A-FE2B1975FF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4DAC6243-DA4E-4FCF-9809-25EC7B85770D}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="326">
   <si>
     <t>property_name</t>
   </si>
@@ -561,9 +561,6 @@
   </si>
   <si>
     <t>ANGGREK-36</t>
-  </si>
-  <si>
-    <t>Note : di excel ada R-37</t>
   </si>
   <si>
     <t>PONDOK JEPUN</t>
@@ -1375,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{294A9EED-A0F6-4205-BF9A-CF10CBF56B66}">
   <dimension ref="A1:S174"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="P92" sqref="P92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1404,25 +1401,25 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>322</v>
+      </c>
+      <c r="F1" t="s">
         <v>323</v>
       </c>
-      <c r="F1" t="s">
-        <v>324</v>
-      </c>
       <c r="G1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -1431,7 +1428,7 @@
         <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="K1" t="s">
         <v>4</v>
@@ -1446,19 +1443,19 @@
         <v>7</v>
       </c>
       <c r="O1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P1" t="s">
         <v>8</v>
       </c>
       <c r="Q1" t="s">
+        <v>317</v>
+      </c>
+      <c r="R1" t="s">
         <v>318</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>319</v>
-      </c>
-      <c r="S1" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -1508,7 +1505,7 @@
         <v>3326</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -1558,7 +1555,7 @@
         <v>550</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -1608,7 +1605,7 @@
         <v>3975</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -1658,7 +1655,7 @@
         <v>9142</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -1708,7 +1705,7 @@
         <v>588</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1758,7 +1755,7 @@
         <v>1757</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -1808,7 +1805,7 @@
         <v>879</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -1858,7 +1855,7 @@
         <v>200</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -1908,7 +1905,7 @@
         <v>1815</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1958,7 +1955,7 @@
         <v>3819</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -2008,7 +2005,7 @@
         <v>254</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -2055,7 +2052,7 @@
         <v>174</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -2105,7 +2102,7 @@
         <v>301</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -2155,7 +2152,7 @@
         <v>5751</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -2202,7 +2199,7 @@
         <v>3347</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
@@ -2252,7 +2249,7 @@
         <v>3355</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -2302,7 +2299,7 @@
         <v>2604</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -2349,7 +2346,7 @@
         <v>28426</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -2396,7 +2393,7 @@
         <v>2851</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
@@ -2443,7 +2440,7 @@
         <v>5375</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -2490,7 +2487,7 @@
         <v>22</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -2537,7 +2534,7 @@
         <v>2520</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -2587,7 +2584,7 @@
         <v>7562</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -2637,7 +2634,7 @@
         <v>8030</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -2687,7 +2684,7 @@
         <v>4347</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
@@ -2737,7 +2734,7 @@
         <v>3549</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -2787,7 +2784,7 @@
         <v>8634</v>
       </c>
       <c r="S28" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
@@ -2837,7 +2834,7 @@
         <v>4654</v>
       </c>
       <c r="S29" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -2887,7 +2884,7 @@
         <v>2947</v>
       </c>
       <c r="S30" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -2934,7 +2931,7 @@
         <v>5738</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
@@ -2981,7 +2978,7 @@
         <v>3957</v>
       </c>
       <c r="S32" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
@@ -3028,7 +3025,7 @@
         <v>3666</v>
       </c>
       <c r="S33" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
@@ -3078,7 +3075,7 @@
         <v>5257</v>
       </c>
       <c r="S34" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
@@ -3128,7 +3125,7 @@
         <v>3891</v>
       </c>
       <c r="S35" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -3178,7 +3175,7 @@
         <v>3120</v>
       </c>
       <c r="S36" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
@@ -3228,7 +3225,7 @@
         <v>12596</v>
       </c>
       <c r="S37" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
@@ -3278,7 +3275,7 @@
         <v>5572</v>
       </c>
       <c r="S38" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
@@ -3328,7 +3325,7 @@
         <v>2837</v>
       </c>
       <c r="S39" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
@@ -3378,7 +3375,7 @@
         <v>5206</v>
       </c>
       <c r="S40" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
@@ -3428,7 +3425,7 @@
         <v>1996</v>
       </c>
       <c r="S41" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
@@ -3475,7 +3472,7 @@
         <v>5020</v>
       </c>
       <c r="S42" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
@@ -3525,7 +3522,7 @@
         <v>3753</v>
       </c>
       <c r="S43" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
@@ -3575,7 +3572,7 @@
         <v>3347</v>
       </c>
       <c r="S44" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
@@ -3625,7 +3622,7 @@
         <v>5994</v>
       </c>
       <c r="S45" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
@@ -3675,7 +3672,7 @@
         <v>229</v>
       </c>
       <c r="S46" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
@@ -3725,7 +3722,7 @@
         <v>2265</v>
       </c>
       <c r="S47" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
@@ -3772,7 +3769,7 @@
         <v>2616</v>
       </c>
       <c r="S48" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
@@ -3822,7 +3819,7 @@
         <v>2249</v>
       </c>
       <c r="S49" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
@@ -3869,7 +3866,7 @@
         <v>803</v>
       </c>
       <c r="S50" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
@@ -3916,7 +3913,7 @@
         <v>3699</v>
       </c>
       <c r="S51" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
@@ -3966,7 +3963,7 @@
         <v>8845</v>
       </c>
       <c r="S52" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
@@ -4013,7 +4010,7 @@
         <v>4084</v>
       </c>
       <c r="S53" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
@@ -4063,7 +4060,7 @@
         <v>3423</v>
       </c>
       <c r="S54" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
@@ -4113,7 +4110,7 @@
         <v>8439</v>
       </c>
       <c r="S55" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
@@ -4163,7 +4160,7 @@
         <v>5942</v>
       </c>
       <c r="S56" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
@@ -4213,7 +4210,7 @@
         <v>3727</v>
       </c>
       <c r="S57" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
@@ -4260,7 +4257,7 @@
         <v>4491</v>
       </c>
       <c r="S58" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
@@ -4307,7 +4304,7 @@
         <v>3514</v>
       </c>
       <c r="S59" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
@@ -4354,7 +4351,7 @@
         <v>2831</v>
       </c>
       <c r="S60" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
@@ -4401,7 +4398,7 @@
         <v>3591</v>
       </c>
       <c r="S61" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
@@ -4448,7 +4445,7 @@
         <v>3143</v>
       </c>
       <c r="S62" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
@@ -4495,7 +4492,7 @@
         <v>156</v>
       </c>
       <c r="S63" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
@@ -4545,7 +4542,7 @@
         <v>6177</v>
       </c>
       <c r="S64" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
@@ -4595,7 +4592,7 @@
         <v>4025</v>
       </c>
       <c r="S65" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
@@ -4642,7 +4639,7 @@
         <v>9430</v>
       </c>
       <c r="S66" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
@@ -4692,7 +4689,7 @@
         <v>1799</v>
       </c>
       <c r="S67" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
@@ -4739,7 +4736,7 @@
         <v>2440</v>
       </c>
       <c r="S68" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
@@ -4786,7 +4783,7 @@
         <v>4656</v>
       </c>
       <c r="S69" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
@@ -4833,7 +4830,7 @@
         <v>3588</v>
       </c>
       <c r="S70" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
@@ -4880,7 +4877,7 @@
         <v>3026</v>
       </c>
       <c r="S71" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
@@ -4927,7 +4924,7 @@
         <v>157</v>
       </c>
       <c r="S72" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
@@ -4974,7 +4971,7 @@
         <v>3658</v>
       </c>
       <c r="S73" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.25">
@@ -5024,7 +5021,7 @@
         <v>2886</v>
       </c>
       <c r="S74" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
@@ -5074,7 +5071,7 @@
         <v>5761</v>
       </c>
       <c r="S75" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.25">
@@ -5121,7 +5118,7 @@
         <v>4165</v>
       </c>
       <c r="S76" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.25">
@@ -5168,7 +5165,7 @@
         <v>8057</v>
       </c>
       <c r="S77" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.25">
@@ -5218,7 +5215,7 @@
         <v>5102</v>
       </c>
       <c r="S78" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.25">
@@ -5265,7 +5262,7 @@
         <v>4847</v>
       </c>
       <c r="S79" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.25">
@@ -5312,7 +5309,7 @@
         <v>5082</v>
       </c>
       <c r="S80" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.25">
@@ -5362,7 +5359,7 @@
         <v>411</v>
       </c>
       <c r="S81" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.25">
@@ -5409,7 +5406,7 @@
         <v>4842</v>
       </c>
       <c r="S82" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
@@ -5459,7 +5456,7 @@
         <v>3753</v>
       </c>
       <c r="S83" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.25">
@@ -5509,7 +5506,7 @@
         <v>5921</v>
       </c>
       <c r="S84" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.25">
@@ -5559,7 +5556,7 @@
         <v>453</v>
       </c>
       <c r="S85" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.25">
@@ -5606,7 +5603,7 @@
         <v>112</v>
       </c>
       <c r="S86" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.25">
@@ -5656,7 +5653,7 @@
         <v>3571</v>
       </c>
       <c r="S87" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.25">
@@ -5706,7 +5703,7 @@
         <v>3654</v>
       </c>
       <c r="S88" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.25">
@@ -5756,7 +5753,7 @@
         <v>436</v>
       </c>
       <c r="S89" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.25">
@@ -5803,7 +5800,7 @@
         <v>5440</v>
       </c>
       <c r="S90" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.25">
@@ -5853,7 +5850,7 @@
         <v>7597</v>
       </c>
       <c r="S91" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.25">
@@ -5903,7 +5900,7 @@
         <v>5479</v>
       </c>
       <c r="S92" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.25">
@@ -5953,7 +5950,7 @@
         <v>4754</v>
       </c>
       <c r="S93" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.25">
@@ -6003,7 +6000,7 @@
         <v>3491</v>
       </c>
       <c r="S94" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.25">
@@ -6053,7 +6050,7 @@
         <v>448</v>
       </c>
       <c r="S95" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.25">
@@ -6100,7 +6097,7 @@
         <v>12526</v>
       </c>
       <c r="S96" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.25">
@@ -6150,7 +6147,7 @@
         <v>762</v>
       </c>
       <c r="S97" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.25">
@@ -6191,13 +6188,13 @@
         <v>38</v>
       </c>
       <c r="P98">
-        <v>895800229561</v>
+        <v>89580229561</v>
       </c>
       <c r="R98">
         <v>1632</v>
       </c>
       <c r="S98" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.25">
@@ -6243,8 +6240,8 @@
       <c r="R99">
         <v>2725</v>
       </c>
-      <c r="S99" t="s">
-        <v>177</v>
+      <c r="S99" s="1" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="100" spans="1:19" x14ac:dyDescent="0.25">
@@ -6252,10 +6249,10 @@
         <v>9</v>
       </c>
       <c r="B100" t="s">
+        <v>177</v>
+      </c>
+      <c r="E100" t="s">
         <v>178</v>
-      </c>
-      <c r="E100" t="s">
-        <v>179</v>
       </c>
       <c r="F100">
         <v>550000</v>
@@ -6282,7 +6279,7 @@
         <v>1</v>
       </c>
       <c r="N100" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O100" t="s">
         <v>14</v>
@@ -6293,16 +6290,19 @@
       <c r="R100">
         <v>2223</v>
       </c>
+      <c r="S100" s="1" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="101" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>9</v>
       </c>
       <c r="B101" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E101" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F101">
         <v>550000</v>
@@ -6329,7 +6329,7 @@
         <v>1</v>
       </c>
       <c r="N101" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O101" t="s">
         <v>14</v>
@@ -6340,16 +6340,19 @@
       <c r="R101">
         <v>3636</v>
       </c>
+      <c r="S101" s="1" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>9</v>
       </c>
       <c r="B102" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E102" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F102">
         <v>550000</v>
@@ -6376,7 +6379,7 @@
         <v>1</v>
       </c>
       <c r="N102" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O102" t="s">
         <v>14</v>
@@ -6387,16 +6390,19 @@
       <c r="R102">
         <v>119</v>
       </c>
+      <c r="S102" s="1" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>9</v>
       </c>
       <c r="B103" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E103" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F103">
         <v>550000</v>
@@ -6423,7 +6429,7 @@
         <v>1</v>
       </c>
       <c r="N103" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O103" t="s">
         <v>14</v>
@@ -6434,16 +6440,19 @@
       <c r="R103">
         <v>45</v>
       </c>
+      <c r="S103" s="1" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>9</v>
       </c>
       <c r="B104" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E104" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F104">
         <v>550000</v>
@@ -6470,7 +6479,7 @@
         <v>1</v>
       </c>
       <c r="N104" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="O104" t="s">
         <v>14</v>
@@ -6481,16 +6490,19 @@
       <c r="R104">
         <v>813</v>
       </c>
+      <c r="S104" s="1" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>9</v>
       </c>
       <c r="B105" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E105" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F105">
         <v>550000</v>
@@ -6517,7 +6529,7 @@
         <v>1</v>
       </c>
       <c r="N105" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O105" t="s">
         <v>14</v>
@@ -6528,16 +6540,19 @@
       <c r="R105">
         <v>6207</v>
       </c>
+      <c r="S105" s="1" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>9</v>
       </c>
       <c r="B106" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E106" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F106">
         <v>550000</v>
@@ -6564,7 +6579,7 @@
         <v>1</v>
       </c>
       <c r="N106" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O106" t="s">
         <v>14</v>
@@ -6575,16 +6590,19 @@
       <c r="R106">
         <v>1329</v>
       </c>
+      <c r="S106" s="1" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>9</v>
       </c>
       <c r="B107" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E107" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F107">
         <v>550000</v>
@@ -6611,7 +6629,7 @@
         <v>1</v>
       </c>
       <c r="N107" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="O107" t="s">
         <v>14</v>
@@ -6622,16 +6640,19 @@
       <c r="R107">
         <v>21371</v>
       </c>
+      <c r="S107" s="1" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>9</v>
       </c>
       <c r="B108" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E108" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F108">
         <v>550000</v>
@@ -6666,16 +6687,19 @@
       <c r="R108">
         <v>98</v>
       </c>
+      <c r="S108" s="1" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="109" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>9</v>
       </c>
       <c r="B109" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E109" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F109">
         <v>550000</v>
@@ -6710,16 +6734,19 @@
       <c r="R109">
         <v>7325</v>
       </c>
+      <c r="S109" s="1" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="110" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>9</v>
       </c>
       <c r="B110" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E110" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F110">
         <v>550000</v>
@@ -6746,7 +6773,7 @@
         <v>1</v>
       </c>
       <c r="N110" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O110" t="s">
         <v>14</v>
@@ -6757,16 +6784,19 @@
       <c r="R110">
         <v>3394</v>
       </c>
+      <c r="S110" s="1" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="111" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>9</v>
       </c>
       <c r="B111" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E111" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F111">
         <v>550000</v>
@@ -6793,7 +6823,7 @@
         <v>1</v>
       </c>
       <c r="N111" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O111" t="s">
         <v>14</v>
@@ -6804,16 +6834,19 @@
       <c r="R111">
         <v>3152</v>
       </c>
+      <c r="S111" s="1" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>9</v>
       </c>
       <c r="B112" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E112" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F112">
         <v>550000</v>
@@ -6840,7 +6873,7 @@
         <v>1</v>
       </c>
       <c r="N112" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O112" t="s">
         <v>14</v>
@@ -6851,16 +6884,19 @@
       <c r="R112">
         <v>7377</v>
       </c>
-    </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S112" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>9</v>
       </c>
       <c r="B113" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E113" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F113">
         <v>550000</v>
@@ -6887,7 +6923,7 @@
         <v>1</v>
       </c>
       <c r="N113" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O113" t="s">
         <v>14</v>
@@ -6898,16 +6934,19 @@
       <c r="R113">
         <v>8571</v>
       </c>
-    </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S113" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>9</v>
       </c>
       <c r="B114" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E114" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F114">
         <v>550000</v>
@@ -6934,7 +6973,7 @@
         <v>1</v>
       </c>
       <c r="N114" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O114" t="s">
         <v>14</v>
@@ -6945,16 +6984,19 @@
       <c r="R114">
         <v>2874</v>
       </c>
-    </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S114" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>9</v>
       </c>
       <c r="B115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E115" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F115">
         <v>550000</v>
@@ -6981,7 +7023,7 @@
         <v>1</v>
       </c>
       <c r="N115" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="O115" t="s">
         <v>14</v>
@@ -6989,16 +7031,22 @@
       <c r="P115" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R115">
+        <v>0</v>
+      </c>
+      <c r="S115" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>9</v>
       </c>
       <c r="B116" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E116" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F116">
         <v>550000</v>
@@ -7025,7 +7073,7 @@
         <v>1</v>
       </c>
       <c r="N116" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="O116" t="s">
         <v>14</v>
@@ -7033,16 +7081,22 @@
       <c r="P116" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R116">
+        <v>0</v>
+      </c>
+      <c r="S116" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>9</v>
       </c>
       <c r="B117" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E117" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F117">
         <v>550000</v>
@@ -7069,7 +7123,7 @@
         <v>1</v>
       </c>
       <c r="N117" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="O117" t="s">
         <v>14</v>
@@ -7077,16 +7131,22 @@
       <c r="P117" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R117">
+        <v>0</v>
+      </c>
+      <c r="S117" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>9</v>
       </c>
       <c r="B118" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E118" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F118">
         <v>550000</v>
@@ -7113,7 +7173,7 @@
         <v>1</v>
       </c>
       <c r="N118" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O118" t="s">
         <v>14</v>
@@ -7121,16 +7181,22 @@
       <c r="P118" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R118">
+        <v>0</v>
+      </c>
+      <c r="S118" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>9</v>
       </c>
       <c r="B119" t="s">
+        <v>210</v>
+      </c>
+      <c r="E119" t="s">
         <v>211</v>
-      </c>
-      <c r="E119" t="s">
-        <v>212</v>
       </c>
       <c r="F119">
         <v>1000000</v>
@@ -7162,16 +7228,22 @@
       <c r="P119" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R119">
+        <v>0</v>
+      </c>
+      <c r="S119" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>9</v>
       </c>
       <c r="B120" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E120" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F120">
         <v>1000000</v>
@@ -7203,16 +7275,22 @@
       <c r="P120" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R120">
+        <v>0</v>
+      </c>
+      <c r="S120" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>9</v>
       </c>
       <c r="B121" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E121" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F121">
         <v>1000000</v>
@@ -7244,16 +7322,22 @@
       <c r="P121" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R121">
+        <v>0</v>
+      </c>
+      <c r="S121" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>9</v>
       </c>
       <c r="B122" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E122" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F122">
         <v>1000000</v>
@@ -7285,16 +7369,22 @@
       <c r="P122" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R122">
+        <v>0</v>
+      </c>
+      <c r="S122" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>9</v>
       </c>
       <c r="B123" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E123" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F123">
         <v>1000000</v>
@@ -7326,16 +7416,22 @@
       <c r="P123" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R123">
+        <v>0</v>
+      </c>
+      <c r="S123" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>9</v>
       </c>
       <c r="B124" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E124" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F124">
         <v>1000000</v>
@@ -7367,16 +7463,22 @@
       <c r="P124" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R124">
+        <v>0</v>
+      </c>
+      <c r="S124" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>9</v>
       </c>
       <c r="B125" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E125" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F125">
         <v>1000000</v>
@@ -7408,16 +7510,22 @@
       <c r="P125" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R125">
+        <v>0</v>
+      </c>
+      <c r="S125" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>9</v>
       </c>
       <c r="B126" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E126" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F126">
         <v>1000000</v>
@@ -7449,16 +7557,22 @@
       <c r="P126" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R126">
+        <v>0</v>
+      </c>
+      <c r="S126" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>9</v>
       </c>
       <c r="B127" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E127" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F127">
         <v>1000000</v>
@@ -7490,16 +7604,22 @@
       <c r="P127" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R127">
+        <v>0</v>
+      </c>
+      <c r="S127" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>9</v>
       </c>
       <c r="B128" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E128" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F128">
         <v>1000000</v>
@@ -7531,16 +7651,22 @@
       <c r="P128" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R128">
+        <v>0</v>
+      </c>
+      <c r="S128" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>9</v>
       </c>
       <c r="B129" t="s">
+        <v>221</v>
+      </c>
+      <c r="E129" t="s">
         <v>222</v>
-      </c>
-      <c r="E129" t="s">
-        <v>223</v>
       </c>
       <c r="F129">
         <v>800000</v>
@@ -7567,7 +7693,7 @@
         <v>1</v>
       </c>
       <c r="N129" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O129" t="s">
         <v>14</v>
@@ -7578,16 +7704,19 @@
       <c r="R129">
         <v>2416</v>
       </c>
-    </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S129" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>9</v>
       </c>
       <c r="B130" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E130" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F130">
         <v>800000</v>
@@ -7614,7 +7743,7 @@
         <v>1</v>
       </c>
       <c r="N130" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O130" t="s">
         <v>14</v>
@@ -7625,16 +7754,19 @@
       <c r="R130">
         <v>3029</v>
       </c>
-    </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S130" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>9</v>
       </c>
       <c r="B131" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E131" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F131">
         <v>800000</v>
@@ -7661,7 +7793,7 @@
         <v>1</v>
       </c>
       <c r="N131" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O131" t="s">
         <v>14</v>
@@ -7672,16 +7804,19 @@
       <c r="R131">
         <v>2609</v>
       </c>
-    </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S131" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>9</v>
       </c>
       <c r="B132" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E132" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F132">
         <v>800000</v>
@@ -7708,7 +7843,7 @@
         <v>1</v>
       </c>
       <c r="N132" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="O132" t="s">
         <v>14</v>
@@ -7719,16 +7854,19 @@
       <c r="R132">
         <v>1918</v>
       </c>
-    </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S132" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>9</v>
       </c>
       <c r="B133" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E133" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F133">
         <v>800000</v>
@@ -7755,7 +7893,7 @@
         <v>1</v>
       </c>
       <c r="N133" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O133" t="s">
         <v>14</v>
@@ -7766,16 +7904,19 @@
       <c r="R133">
         <v>2047</v>
       </c>
-    </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S133" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>9</v>
       </c>
       <c r="B134" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E134" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F134">
         <v>800000</v>
@@ -7802,7 +7943,7 @@
         <v>1</v>
       </c>
       <c r="N134" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O134" t="s">
         <v>14</v>
@@ -7813,16 +7954,19 @@
       <c r="R134">
         <v>4162</v>
       </c>
-    </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S134" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>9</v>
       </c>
       <c r="B135" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E135" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F135">
         <v>800000</v>
@@ -7849,7 +7993,7 @@
         <v>1</v>
       </c>
       <c r="N135" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="O135" t="s">
         <v>14</v>
@@ -7860,16 +8004,19 @@
       <c r="R135">
         <v>1866</v>
       </c>
-    </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S135" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>9</v>
       </c>
       <c r="B136" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E136" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F136">
         <v>800000</v>
@@ -7896,7 +8043,7 @@
         <v>1</v>
       </c>
       <c r="N136" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="O136" t="s">
         <v>14</v>
@@ -7907,16 +8054,19 @@
       <c r="R136">
         <v>972</v>
       </c>
-    </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S136" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>9</v>
       </c>
       <c r="B137" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E137" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F137">
         <v>800000</v>
@@ -7943,7 +8093,7 @@
         <v>1</v>
       </c>
       <c r="N137" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="O137" t="s">
         <v>14</v>
@@ -7954,16 +8104,19 @@
       <c r="R137">
         <v>1440</v>
       </c>
-    </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S137" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>9</v>
       </c>
       <c r="B138" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E138" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F138">
         <v>800000</v>
@@ -7990,7 +8143,7 @@
         <v>1</v>
       </c>
       <c r="N138" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="O138" t="s">
         <v>14</v>
@@ -8001,16 +8154,19 @@
       <c r="R138">
         <v>1560</v>
       </c>
-    </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S138" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>9</v>
       </c>
       <c r="B139" t="s">
+        <v>242</v>
+      </c>
+      <c r="E139" t="s">
         <v>243</v>
-      </c>
-      <c r="E139" t="s">
-        <v>244</v>
       </c>
       <c r="F139">
         <v>800000</v>
@@ -8037,7 +8193,7 @@
         <v>1</v>
       </c>
       <c r="N139" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O139" t="s">
         <v>14</v>
@@ -8048,16 +8204,19 @@
       <c r="R139">
         <v>1644</v>
       </c>
-    </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S139" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>9</v>
       </c>
       <c r="B140" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E140" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F140">
         <v>800000</v>
@@ -8084,7 +8243,7 @@
         <v>1</v>
       </c>
       <c r="N140" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O140" t="s">
         <v>14</v>
@@ -8095,16 +8254,19 @@
       <c r="R140">
         <v>1699</v>
       </c>
-    </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S140" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>9</v>
       </c>
       <c r="B141" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E141" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F141">
         <v>800000</v>
@@ -8131,7 +8293,7 @@
         <v>1</v>
       </c>
       <c r="N141" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="O141" t="s">
         <v>14</v>
@@ -8142,16 +8304,19 @@
       <c r="R141">
         <v>1572</v>
       </c>
-    </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S141" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>9</v>
       </c>
       <c r="B142" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E142" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F142">
         <v>800000</v>
@@ -8178,7 +8343,7 @@
         <v>1</v>
       </c>
       <c r="N142" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O142" t="s">
         <v>14</v>
@@ -8189,16 +8354,19 @@
       <c r="R142">
         <v>8801</v>
       </c>
-    </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S142" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>9</v>
       </c>
       <c r="B143" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E143" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F143">
         <v>800000</v>
@@ -8225,7 +8393,7 @@
         <v>1</v>
       </c>
       <c r="N143" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O143" t="s">
         <v>14</v>
@@ -8236,16 +8404,19 @@
       <c r="R143">
         <v>1870</v>
       </c>
-    </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S143" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>9</v>
       </c>
       <c r="B144" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E144" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F144">
         <v>800000</v>
@@ -8272,7 +8443,7 @@
         <v>1</v>
       </c>
       <c r="N144" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O144" t="s">
         <v>14</v>
@@ -8283,16 +8454,19 @@
       <c r="R144">
         <v>2845</v>
       </c>
-    </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S144" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>9</v>
       </c>
       <c r="B145" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E145" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F145">
         <v>800000</v>
@@ -8319,7 +8493,7 @@
         <v>1</v>
       </c>
       <c r="N145" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="O145" t="s">
         <v>14</v>
@@ -8330,16 +8504,19 @@
       <c r="R145">
         <v>2965</v>
       </c>
-    </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S145" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>9</v>
       </c>
       <c r="B146" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E146" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F146">
         <v>800000</v>
@@ -8366,7 +8543,7 @@
         <v>1</v>
       </c>
       <c r="N146" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="O146" t="s">
         <v>14</v>
@@ -8377,16 +8554,19 @@
       <c r="R146">
         <v>1875</v>
       </c>
-    </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S146" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>9</v>
       </c>
       <c r="B147" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E147" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F147">
         <v>800000</v>
@@ -8413,7 +8593,7 @@
         <v>1</v>
       </c>
       <c r="N147" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="O147" t="s">
         <v>14</v>
@@ -8424,16 +8604,19 @@
       <c r="R147">
         <v>1263</v>
       </c>
-    </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S147" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>9</v>
       </c>
       <c r="B148" t="s">
+        <v>261</v>
+      </c>
+      <c r="E148" t="s">
         <v>262</v>
-      </c>
-      <c r="E148" t="s">
-        <v>263</v>
       </c>
       <c r="F148">
         <v>800000</v>
@@ -8460,7 +8643,7 @@
         <v>1</v>
       </c>
       <c r="N148" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O148" t="s">
         <v>14</v>
@@ -8471,16 +8654,19 @@
       <c r="R148">
         <v>3198</v>
       </c>
-    </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S148" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>9</v>
       </c>
       <c r="B149" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E149" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F149">
         <v>800000</v>
@@ -8507,7 +8693,7 @@
         <v>1</v>
       </c>
       <c r="N149" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O149" t="s">
         <v>14</v>
@@ -8518,16 +8704,19 @@
       <c r="R149">
         <v>1838</v>
       </c>
-    </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S149" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>9</v>
       </c>
       <c r="B150" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E150" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F150">
         <v>800000</v>
@@ -8554,7 +8743,7 @@
         <v>1</v>
       </c>
       <c r="N150" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="O150" t="s">
         <v>14</v>
@@ -8565,16 +8754,19 @@
       <c r="R150">
         <v>1636</v>
       </c>
-    </row>
-    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S150" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>9</v>
       </c>
       <c r="B151" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E151" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F151">
         <v>800000</v>
@@ -8601,7 +8793,7 @@
         <v>1</v>
       </c>
       <c r="N151" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="O151" t="s">
         <v>14</v>
@@ -8612,16 +8804,19 @@
       <c r="R151">
         <v>2925</v>
       </c>
-    </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S151" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>9</v>
       </c>
       <c r="B152" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E152" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F152">
         <v>800000</v>
@@ -8648,7 +8843,7 @@
         <v>1</v>
       </c>
       <c r="N152" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="O152" t="s">
         <v>14</v>
@@ -8659,16 +8854,19 @@
       <c r="R152">
         <v>3426</v>
       </c>
-    </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S152" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>9</v>
       </c>
       <c r="B153" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E153" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F153">
         <v>800000</v>
@@ -8695,7 +8893,7 @@
         <v>1</v>
       </c>
       <c r="N153" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="O153" t="s">
         <v>14</v>
@@ -8706,16 +8904,19 @@
       <c r="R153">
         <v>1383</v>
       </c>
-    </row>
-    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S153" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>9</v>
       </c>
       <c r="B154" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E154" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F154">
         <v>800000</v>
@@ -8742,7 +8943,7 @@
         <v>1</v>
       </c>
       <c r="N154" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="O154" t="s">
         <v>14</v>
@@ -8753,16 +8954,19 @@
       <c r="R154">
         <v>202</v>
       </c>
-    </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S154" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>9</v>
       </c>
       <c r="B155" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E155" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F155">
         <v>800000</v>
@@ -8789,7 +8993,7 @@
         <v>1</v>
       </c>
       <c r="N155" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="O155" t="s">
         <v>14</v>
@@ -8800,16 +9004,19 @@
       <c r="R155">
         <v>197</v>
       </c>
-    </row>
-    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S155" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>9</v>
       </c>
       <c r="B156" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E156" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F156">
         <v>800000</v>
@@ -8836,7 +9043,7 @@
         <v>1</v>
       </c>
       <c r="N156" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="O156" t="s">
         <v>14</v>
@@ -8847,16 +9054,19 @@
       <c r="R156">
         <v>359</v>
       </c>
-    </row>
-    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S156" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>9</v>
       </c>
       <c r="B157" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E157" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F157">
         <v>800000</v>
@@ -8883,7 +9093,7 @@
         <v>1</v>
       </c>
       <c r="N157" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O157" t="s">
         <v>14</v>
@@ -8894,16 +9104,19 @@
       <c r="R157">
         <v>2012</v>
       </c>
-    </row>
-    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S157" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>9</v>
       </c>
       <c r="B158" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E158" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F158">
         <v>800000</v>
@@ -8930,7 +9143,7 @@
         <v>1</v>
       </c>
       <c r="N158" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="O158" t="s">
         <v>14</v>
@@ -8941,16 +9154,19 @@
       <c r="R158">
         <v>2381</v>
       </c>
-    </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S158" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>9</v>
       </c>
       <c r="B159" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E159" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F159">
         <v>800000</v>
@@ -8977,7 +9193,7 @@
         <v>1</v>
       </c>
       <c r="N159" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="O159" t="s">
         <v>14</v>
@@ -8988,16 +9204,19 @@
       <c r="R159">
         <v>1479</v>
       </c>
-    </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S159" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>9</v>
       </c>
       <c r="B160" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E160" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F160">
         <v>800000</v>
@@ -9024,7 +9243,7 @@
         <v>1</v>
       </c>
       <c r="N160" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="O160" t="s">
         <v>14</v>
@@ -9035,16 +9254,19 @@
       <c r="R160">
         <v>668</v>
       </c>
-    </row>
-    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S160" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="161" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>9</v>
       </c>
       <c r="B161" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E161" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F161">
         <v>800000</v>
@@ -9071,7 +9293,7 @@
         <v>1</v>
       </c>
       <c r="N161" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O161" t="s">
         <v>14</v>
@@ -9082,16 +9304,19 @@
       <c r="R161">
         <v>3198</v>
       </c>
-    </row>
-    <row r="162" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S161" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="162" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>9</v>
       </c>
       <c r="B162" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E162" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F162">
         <v>800000</v>
@@ -9118,7 +9343,7 @@
         <v>1</v>
       </c>
       <c r="N162" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="O162" t="s">
         <v>14</v>
@@ -9129,16 +9354,19 @@
       <c r="R162">
         <v>1231</v>
       </c>
-    </row>
-    <row r="163" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S162" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="163" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>9</v>
       </c>
       <c r="B163" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E163" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F163">
         <v>800000</v>
@@ -9165,7 +9393,7 @@
         <v>1</v>
       </c>
       <c r="N163" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="O163" t="s">
         <v>14</v>
@@ -9176,16 +9404,19 @@
       <c r="R163">
         <v>2476</v>
       </c>
-    </row>
-    <row r="164" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S163" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="164" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>9</v>
       </c>
       <c r="B164" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E164" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F164">
         <v>800000</v>
@@ -9212,7 +9443,7 @@
         <v>1</v>
       </c>
       <c r="N164" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="O164" t="s">
         <v>14</v>
@@ -9223,16 +9454,19 @@
       <c r="R164">
         <v>3437</v>
       </c>
-    </row>
-    <row r="165" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S164" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="165" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>9</v>
       </c>
       <c r="B165" t="s">
+        <v>295</v>
+      </c>
+      <c r="E165" t="s">
         <v>296</v>
-      </c>
-      <c r="E165" t="s">
-        <v>297</v>
       </c>
       <c r="F165">
         <v>850000</v>
@@ -9259,7 +9493,7 @@
         <v>1</v>
       </c>
       <c r="N165" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="O165" t="s">
         <v>14</v>
@@ -9270,16 +9504,19 @@
       <c r="R165">
         <v>2021</v>
       </c>
-    </row>
-    <row r="166" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S165" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="166" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>9</v>
       </c>
       <c r="B166" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E166" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F166">
         <v>850000</v>
@@ -9306,7 +9543,7 @@
         <v>1</v>
       </c>
       <c r="N166" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="O166" t="s">
         <v>14</v>
@@ -9317,16 +9554,19 @@
       <c r="R166">
         <v>763</v>
       </c>
-    </row>
-    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S166" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="167" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>9</v>
       </c>
       <c r="B167" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E167" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F167">
         <v>850000</v>
@@ -9353,7 +9593,7 @@
         <v>1</v>
       </c>
       <c r="N167" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="O167" t="s">
         <v>14</v>
@@ -9364,16 +9604,19 @@
       <c r="R167">
         <v>1458</v>
       </c>
-    </row>
-    <row r="168" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S167" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="168" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>9</v>
       </c>
       <c r="B168" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E168" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F168">
         <v>850000</v>
@@ -9400,7 +9643,7 @@
         <v>1</v>
       </c>
       <c r="N168" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="O168" t="s">
         <v>14</v>
@@ -9411,16 +9654,19 @@
       <c r="R168">
         <v>1385</v>
       </c>
-    </row>
-    <row r="169" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S168" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="169" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>9</v>
       </c>
       <c r="B169" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E169" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F169">
         <v>850000</v>
@@ -9447,7 +9693,7 @@
         <v>1</v>
       </c>
       <c r="N169" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="O169" t="s">
         <v>14</v>
@@ -9458,16 +9704,19 @@
       <c r="R169">
         <v>3349</v>
       </c>
-    </row>
-    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S169" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="170" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>9</v>
       </c>
       <c r="B170" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E170" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F170">
         <v>850000</v>
@@ -9494,7 +9743,7 @@
         <v>1</v>
       </c>
       <c r="N170" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="O170" t="s">
         <v>14</v>
@@ -9505,16 +9754,19 @@
       <c r="R170">
         <v>1288</v>
       </c>
-    </row>
-    <row r="171" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S170" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="171" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>9</v>
       </c>
       <c r="B171" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E171" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F171">
         <v>850000</v>
@@ -9541,7 +9793,7 @@
         <v>1</v>
       </c>
       <c r="N171" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="O171" t="s">
         <v>14</v>
@@ -9552,16 +9804,19 @@
       <c r="R171">
         <v>3511</v>
       </c>
-    </row>
-    <row r="172" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S171" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="172" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>9</v>
       </c>
       <c r="B172" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E172" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F172">
         <v>850000</v>
@@ -9588,7 +9843,7 @@
         <v>1</v>
       </c>
       <c r="N172" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="O172" t="s">
         <v>14</v>
@@ -9599,16 +9854,19 @@
       <c r="R172">
         <v>806</v>
       </c>
-    </row>
-    <row r="173" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S172" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="173" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>9</v>
       </c>
       <c r="B173" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E173" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F173">
         <v>850000</v>
@@ -9635,7 +9893,7 @@
         <v>1</v>
       </c>
       <c r="N173" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="O173" t="s">
         <v>14</v>
@@ -9646,16 +9904,19 @@
       <c r="R173">
         <v>1166</v>
       </c>
-    </row>
-    <row r="174" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S173" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="174" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>9</v>
       </c>
       <c r="B174" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E174" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F174">
         <v>850000</v>
@@ -9682,7 +9943,7 @@
         <v>1</v>
       </c>
       <c r="N174" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O174" t="s">
         <v>14</v>
@@ -9692,12 +9953,16 @@
       </c>
       <c r="R174">
         <v>1644</v>
+      </c>
+      <c r="S174" s="1" t="s">
+        <v>320</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="S2" r:id="rId1" xr:uid="{2FF307E4-C3FA-4F93-8793-A61B89C2B444}"/>
     <hyperlink ref="S3:S98" r:id="rId2" display="admin@example.com" xr:uid="{284699D7-3B73-42A0-8AE8-6E9F0367C465}"/>
+    <hyperlink ref="S99:S174" r:id="rId3" display="admin@example.com" xr:uid="{5595FEF3-FBD4-4F5D-B1D8-71AF2D0D72AA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: bug room details page with tenant assignment, status management, and billing history, supported by a new room API and tenant selection modal.
</commit_message>
<xml_diff>
--- a/docs/clean.xlsx
+++ b/docs/clean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gunaw\KostMan\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FEA1A6-8FCF-49F8-9C8A-FE2B1975FF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7BB523-7CF0-406E-AE46-92513CBC8C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4DAC6243-DA4E-4FCF-9809-25EC7B85770D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{4DAC6243-DA4E-4FCF-9809-25EC7B85770D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1372,34 +1372,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{294A9EED-A0F6-4205-BF9A-CF10CBF56B66}">
   <dimension ref="A1:S174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="P92" sqref="P92"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:Q174"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.81640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>324</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1501,6 +1501,9 @@
       <c r="P2">
         <v>81231275192</v>
       </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
       <c r="R2">
         <v>3326</v>
       </c>
@@ -1508,7 +1511,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1551,6 +1554,9 @@
       <c r="P3">
         <v>85855473307</v>
       </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
       <c r="R3">
         <v>550</v>
       </c>
@@ -1558,7 +1564,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1601,6 +1607,9 @@
       <c r="P4">
         <v>83893380147</v>
       </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
       <c r="R4">
         <v>3975</v>
       </c>
@@ -1608,7 +1617,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1651,6 +1660,9 @@
       <c r="P5">
         <v>81558369157</v>
       </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
       <c r="R5">
         <v>9142</v>
       </c>
@@ -1658,7 +1670,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1701,6 +1713,9 @@
       <c r="P6">
         <v>87853951575</v>
       </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
       <c r="R6">
         <v>588</v>
       </c>
@@ -1708,7 +1723,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1751,6 +1766,9 @@
       <c r="P7">
         <v>82247625007</v>
       </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
       <c r="R7">
         <v>1757</v>
       </c>
@@ -1758,7 +1776,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1801,6 +1819,9 @@
       <c r="P8">
         <v>85865993828</v>
       </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
       <c r="R8">
         <v>879</v>
       </c>
@@ -1808,7 +1829,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1851,6 +1872,9 @@
       <c r="P9">
         <v>81354823520</v>
       </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
       <c r="R9">
         <v>200</v>
       </c>
@@ -1858,7 +1882,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1901,6 +1925,9 @@
       <c r="P10">
         <v>87836736583</v>
       </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
       <c r="R10">
         <v>1815</v>
       </c>
@@ -1908,7 +1935,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1951,6 +1978,9 @@
       <c r="P11">
         <v>81996371243</v>
       </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
       <c r="R11">
         <v>3819</v>
       </c>
@@ -1958,7 +1988,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2001,6 +2031,9 @@
       <c r="P12">
         <v>81332146140</v>
       </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
       <c r="R12">
         <v>254</v>
       </c>
@@ -2008,7 +2041,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -2048,6 +2081,9 @@
       <c r="P13" t="s">
         <v>38</v>
       </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
       <c r="R13">
         <v>174</v>
       </c>
@@ -2055,7 +2091,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -2098,6 +2134,9 @@
       <c r="P14">
         <v>87816007872</v>
       </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
       <c r="R14">
         <v>301</v>
       </c>
@@ -2105,7 +2144,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -2148,6 +2187,9 @@
       <c r="P15">
         <v>8754685763</v>
       </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
       <c r="R15">
         <v>5751</v>
       </c>
@@ -2155,7 +2197,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -2195,6 +2237,9 @@
       <c r="P16">
         <v>81231924248</v>
       </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
       <c r="R16">
         <v>3347</v>
       </c>
@@ -2202,7 +2247,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -2245,6 +2290,9 @@
       <c r="P17">
         <v>85337854431</v>
       </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
       <c r="R17">
         <v>3355</v>
       </c>
@@ -2252,7 +2300,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -2295,6 +2343,9 @@
       <c r="P18">
         <v>87828385427</v>
       </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
       <c r="R18">
         <v>2604</v>
       </c>
@@ -2302,7 +2353,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -2342,6 +2393,9 @@
       <c r="P19" t="s">
         <v>38</v>
       </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
       <c r="R19">
         <v>28426</v>
       </c>
@@ -2349,7 +2403,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -2389,6 +2443,9 @@
       <c r="P20" t="s">
         <v>38</v>
       </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
       <c r="R20">
         <v>2851</v>
       </c>
@@ -2396,7 +2453,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -2436,6 +2493,9 @@
       <c r="P21" t="s">
         <v>38</v>
       </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
       <c r="R21">
         <v>5375</v>
       </c>
@@ -2443,7 +2503,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -2483,6 +2543,9 @@
       <c r="P22" t="s">
         <v>38</v>
       </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
       <c r="R22">
         <v>22</v>
       </c>
@@ -2490,7 +2553,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -2530,6 +2593,9 @@
       <c r="P23" t="s">
         <v>38</v>
       </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
       <c r="R23">
         <v>2520</v>
       </c>
@@ -2537,7 +2603,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -2580,6 +2646,9 @@
       <c r="P24" t="s">
         <v>57</v>
       </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
       <c r="R24">
         <v>7562</v>
       </c>
@@ -2587,7 +2656,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -2630,6 +2699,9 @@
       <c r="P25" t="s">
         <v>57</v>
       </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
       <c r="R25">
         <v>8030</v>
       </c>
@@ -2637,7 +2709,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -2680,6 +2752,9 @@
       <c r="P26" t="s">
         <v>57</v>
       </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
       <c r="R26">
         <v>4347</v>
       </c>
@@ -2687,7 +2762,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -2730,6 +2805,9 @@
       <c r="P27" t="s">
         <v>57</v>
       </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
       <c r="R27">
         <v>3549</v>
       </c>
@@ -2737,7 +2815,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -2780,6 +2858,9 @@
       <c r="P28" t="s">
         <v>57</v>
       </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
       <c r="R28">
         <v>8634</v>
       </c>
@@ -2787,7 +2868,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -2830,6 +2911,9 @@
       <c r="P29" t="s">
         <v>57</v>
       </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
       <c r="R29">
         <v>4654</v>
       </c>
@@ -2837,7 +2921,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -2880,6 +2964,9 @@
       <c r="P30" t="s">
         <v>57</v>
       </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
       <c r="R30">
         <v>2947</v>
       </c>
@@ -2887,7 +2974,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -2927,6 +3014,9 @@
       <c r="P31" t="s">
         <v>38</v>
       </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
       <c r="R31">
         <v>5738</v>
       </c>
@@ -2934,7 +3024,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -2974,6 +3064,9 @@
       <c r="P32" t="s">
         <v>38</v>
       </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
       <c r="R32">
         <v>3957</v>
       </c>
@@ -2981,7 +3074,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -3021,6 +3114,9 @@
       <c r="P33" t="s">
         <v>38</v>
       </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
       <c r="R33">
         <v>3666</v>
       </c>
@@ -3028,7 +3124,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -3071,6 +3167,9 @@
       <c r="P34" t="s">
         <v>57</v>
       </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
       <c r="R34">
         <v>5257</v>
       </c>
@@ -3078,7 +3177,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -3121,6 +3220,9 @@
       <c r="P35" t="s">
         <v>57</v>
       </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
       <c r="R35">
         <v>3891</v>
       </c>
@@ -3128,7 +3230,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -3171,6 +3273,9 @@
       <c r="P36" t="s">
         <v>57</v>
       </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
       <c r="R36">
         <v>3120</v>
       </c>
@@ -3178,7 +3283,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -3221,6 +3326,9 @@
       <c r="P37" t="s">
         <v>57</v>
       </c>
+      <c r="Q37">
+        <v>0</v>
+      </c>
       <c r="R37">
         <v>12596</v>
       </c>
@@ -3228,7 +3336,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -3271,6 +3379,9 @@
       <c r="P38" t="s">
         <v>57</v>
       </c>
+      <c r="Q38">
+        <v>0</v>
+      </c>
       <c r="R38">
         <v>5572</v>
       </c>
@@ -3278,7 +3389,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -3321,6 +3432,9 @@
       <c r="P39" t="s">
         <v>57</v>
       </c>
+      <c r="Q39">
+        <v>0</v>
+      </c>
       <c r="R39">
         <v>2837</v>
       </c>
@@ -3328,7 +3442,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -3371,6 +3485,9 @@
       <c r="P40" t="s">
         <v>57</v>
       </c>
+      <c r="Q40">
+        <v>0</v>
+      </c>
       <c r="R40">
         <v>5206</v>
       </c>
@@ -3378,7 +3495,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -3421,6 +3538,9 @@
       <c r="P41" t="s">
         <v>57</v>
       </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
       <c r="R41">
         <v>1996</v>
       </c>
@@ -3428,7 +3548,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -3468,6 +3588,9 @@
       <c r="P42" t="s">
         <v>38</v>
       </c>
+      <c r="Q42">
+        <v>0</v>
+      </c>
       <c r="R42">
         <v>5020</v>
       </c>
@@ -3475,7 +3598,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -3518,6 +3641,9 @@
       <c r="P43" t="s">
         <v>57</v>
       </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
       <c r="R43">
         <v>3753</v>
       </c>
@@ -3525,7 +3651,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>9</v>
       </c>
@@ -3568,6 +3694,9 @@
       <c r="P44" t="s">
         <v>57</v>
       </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
       <c r="R44">
         <v>3347</v>
       </c>
@@ -3575,7 +3704,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -3618,6 +3747,9 @@
       <c r="P45" t="s">
         <v>57</v>
       </c>
+      <c r="Q45">
+        <v>0</v>
+      </c>
       <c r="R45">
         <v>5994</v>
       </c>
@@ -3625,7 +3757,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -3668,6 +3800,9 @@
       <c r="P46" t="s">
         <v>57</v>
       </c>
+      <c r="Q46">
+        <v>0</v>
+      </c>
       <c r="R46">
         <v>229</v>
       </c>
@@ -3675,7 +3810,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -3718,6 +3853,9 @@
       <c r="P47" t="s">
         <v>57</v>
       </c>
+      <c r="Q47">
+        <v>0</v>
+      </c>
       <c r="R47">
         <v>2265</v>
       </c>
@@ -3725,7 +3863,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -3765,6 +3903,9 @@
       <c r="P48" t="s">
         <v>38</v>
       </c>
+      <c r="Q48">
+        <v>0</v>
+      </c>
       <c r="R48">
         <v>2616</v>
       </c>
@@ -3772,7 +3913,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -3815,6 +3956,9 @@
       <c r="P49" t="s">
         <v>57</v>
       </c>
+      <c r="Q49">
+        <v>0</v>
+      </c>
       <c r="R49">
         <v>2249</v>
       </c>
@@ -3822,7 +3966,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -3862,6 +4006,9 @@
       <c r="P50" t="s">
         <v>38</v>
       </c>
+      <c r="Q50">
+        <v>0</v>
+      </c>
       <c r="R50">
         <v>803</v>
       </c>
@@ -3869,7 +4016,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>9</v>
       </c>
@@ -3909,6 +4056,9 @@
       <c r="P51" t="s">
         <v>38</v>
       </c>
+      <c r="Q51">
+        <v>0</v>
+      </c>
       <c r="R51">
         <v>3699</v>
       </c>
@@ -3916,7 +4066,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>9</v>
       </c>
@@ -3959,6 +4109,9 @@
       <c r="P52" t="s">
         <v>57</v>
       </c>
+      <c r="Q52">
+        <v>0</v>
+      </c>
       <c r="R52">
         <v>8845</v>
       </c>
@@ -3966,7 +4119,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>9</v>
       </c>
@@ -4006,6 +4159,9 @@
       <c r="P53" t="s">
         <v>38</v>
       </c>
+      <c r="Q53">
+        <v>0</v>
+      </c>
       <c r="R53">
         <v>4084</v>
       </c>
@@ -4013,7 +4169,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>9</v>
       </c>
@@ -4056,6 +4212,9 @@
       <c r="P54" t="s">
         <v>57</v>
       </c>
+      <c r="Q54">
+        <v>0</v>
+      </c>
       <c r="R54">
         <v>3423</v>
       </c>
@@ -4063,7 +4222,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>9</v>
       </c>
@@ -4106,6 +4265,9 @@
       <c r="P55" t="s">
         <v>57</v>
       </c>
+      <c r="Q55">
+        <v>0</v>
+      </c>
       <c r="R55">
         <v>8439</v>
       </c>
@@ -4113,7 +4275,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>9</v>
       </c>
@@ -4156,6 +4318,9 @@
       <c r="P56" t="s">
         <v>57</v>
       </c>
+      <c r="Q56">
+        <v>0</v>
+      </c>
       <c r="R56">
         <v>5942</v>
       </c>
@@ -4163,7 +4328,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>9</v>
       </c>
@@ -4206,6 +4371,9 @@
       <c r="P57" t="s">
         <v>57</v>
       </c>
+      <c r="Q57">
+        <v>0</v>
+      </c>
       <c r="R57">
         <v>3727</v>
       </c>
@@ -4213,7 +4381,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>9</v>
       </c>
@@ -4253,6 +4421,9 @@
       <c r="P58" t="s">
         <v>38</v>
       </c>
+      <c r="Q58">
+        <v>0</v>
+      </c>
       <c r="R58">
         <v>4491</v>
       </c>
@@ -4260,7 +4431,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>9</v>
       </c>
@@ -4300,6 +4471,9 @@
       <c r="P59" t="s">
         <v>38</v>
       </c>
+      <c r="Q59">
+        <v>0</v>
+      </c>
       <c r="R59">
         <v>3514</v>
       </c>
@@ -4307,7 +4481,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>9</v>
       </c>
@@ -4347,6 +4521,9 @@
       <c r="P60" t="s">
         <v>38</v>
       </c>
+      <c r="Q60">
+        <v>0</v>
+      </c>
       <c r="R60">
         <v>2831</v>
       </c>
@@ -4354,7 +4531,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>9</v>
       </c>
@@ -4394,6 +4571,9 @@
       <c r="P61" t="s">
         <v>38</v>
       </c>
+      <c r="Q61">
+        <v>0</v>
+      </c>
       <c r="R61">
         <v>3591</v>
       </c>
@@ -4401,7 +4581,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>9</v>
       </c>
@@ -4441,6 +4621,9 @@
       <c r="P62" t="s">
         <v>38</v>
       </c>
+      <c r="Q62">
+        <v>0</v>
+      </c>
       <c r="R62">
         <v>3143</v>
       </c>
@@ -4448,7 +4631,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>9</v>
       </c>
@@ -4488,6 +4671,9 @@
       <c r="P63" t="s">
         <v>38</v>
       </c>
+      <c r="Q63">
+        <v>0</v>
+      </c>
       <c r="R63">
         <v>156</v>
       </c>
@@ -4495,7 +4681,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>9</v>
       </c>
@@ -4538,6 +4724,9 @@
       <c r="P64">
         <v>82236706906</v>
       </c>
+      <c r="Q64">
+        <v>0</v>
+      </c>
       <c r="R64">
         <v>6177</v>
       </c>
@@ -4545,7 +4734,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>9</v>
       </c>
@@ -4588,6 +4777,9 @@
       <c r="P65">
         <v>85784669266</v>
       </c>
+      <c r="Q65">
+        <v>0</v>
+      </c>
       <c r="R65">
         <v>4025</v>
       </c>
@@ -4595,7 +4787,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>9</v>
       </c>
@@ -4635,6 +4827,9 @@
       <c r="P66" t="s">
         <v>38</v>
       </c>
+      <c r="Q66">
+        <v>0</v>
+      </c>
       <c r="R66">
         <v>9430</v>
       </c>
@@ -4642,7 +4837,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>9</v>
       </c>
@@ -4685,6 +4880,9 @@
       <c r="P67">
         <v>82342510369</v>
       </c>
+      <c r="Q67">
+        <v>0</v>
+      </c>
       <c r="R67">
         <v>1799</v>
       </c>
@@ -4692,7 +4890,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>9</v>
       </c>
@@ -4732,6 +4930,9 @@
       <c r="P68" t="s">
         <v>38</v>
       </c>
+      <c r="Q68">
+        <v>0</v>
+      </c>
       <c r="R68">
         <v>2440</v>
       </c>
@@ -4739,7 +4940,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>9</v>
       </c>
@@ -4779,6 +4980,9 @@
       <c r="P69" t="s">
         <v>38</v>
       </c>
+      <c r="Q69">
+        <v>0</v>
+      </c>
       <c r="R69">
         <v>4656</v>
       </c>
@@ -4786,7 +4990,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>9</v>
       </c>
@@ -4826,6 +5030,9 @@
       <c r="P70" t="s">
         <v>38</v>
       </c>
+      <c r="Q70">
+        <v>0</v>
+      </c>
       <c r="R70">
         <v>3588</v>
       </c>
@@ -4833,7 +5040,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>9</v>
       </c>
@@ -4873,6 +5080,9 @@
       <c r="P71" t="s">
         <v>38</v>
       </c>
+      <c r="Q71">
+        <v>0</v>
+      </c>
       <c r="R71">
         <v>3026</v>
       </c>
@@ -4880,7 +5090,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>9</v>
       </c>
@@ -4920,6 +5130,9 @@
       <c r="P72" t="s">
         <v>38</v>
       </c>
+      <c r="Q72">
+        <v>0</v>
+      </c>
       <c r="R72">
         <v>157</v>
       </c>
@@ -4927,7 +5140,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>9</v>
       </c>
@@ -4967,6 +5180,9 @@
       <c r="P73" t="s">
         <v>38</v>
       </c>
+      <c r="Q73">
+        <v>0</v>
+      </c>
       <c r="R73">
         <v>3658</v>
       </c>
@@ -4974,7 +5190,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>9</v>
       </c>
@@ -5017,6 +5233,9 @@
       <c r="P74">
         <v>81529617174</v>
       </c>
+      <c r="Q74">
+        <v>0</v>
+      </c>
       <c r="R74">
         <v>2886</v>
       </c>
@@ -5024,7 +5243,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>9</v>
       </c>
@@ -5067,6 +5286,9 @@
       <c r="P75">
         <v>87752954844</v>
       </c>
+      <c r="Q75">
+        <v>0</v>
+      </c>
       <c r="R75">
         <v>5761</v>
       </c>
@@ -5074,7 +5296,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>9</v>
       </c>
@@ -5114,6 +5336,9 @@
       <c r="P76" t="s">
         <v>38</v>
       </c>
+      <c r="Q76">
+        <v>0</v>
+      </c>
       <c r="R76">
         <v>4165</v>
       </c>
@@ -5121,7 +5346,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>9</v>
       </c>
@@ -5161,6 +5386,9 @@
       <c r="P77">
         <v>87776741842</v>
       </c>
+      <c r="Q77">
+        <v>0</v>
+      </c>
       <c r="R77">
         <v>8057</v>
       </c>
@@ -5168,7 +5396,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>9</v>
       </c>
@@ -5211,6 +5439,9 @@
       <c r="P78">
         <v>83150942026</v>
       </c>
+      <c r="Q78">
+        <v>0</v>
+      </c>
       <c r="R78">
         <v>5102</v>
       </c>
@@ -5218,7 +5449,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>9</v>
       </c>
@@ -5258,6 +5489,9 @@
       <c r="P79" t="s">
         <v>38</v>
       </c>
+      <c r="Q79">
+        <v>0</v>
+      </c>
       <c r="R79">
         <v>4847</v>
       </c>
@@ -5265,7 +5499,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>9</v>
       </c>
@@ -5305,6 +5539,9 @@
       <c r="P80" t="s">
         <v>38</v>
       </c>
+      <c r="Q80">
+        <v>0</v>
+      </c>
       <c r="R80">
         <v>5082</v>
       </c>
@@ -5312,7 +5549,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>9</v>
       </c>
@@ -5355,6 +5592,9 @@
       <c r="P81">
         <v>83870733139</v>
       </c>
+      <c r="Q81">
+        <v>0</v>
+      </c>
       <c r="R81">
         <v>411</v>
       </c>
@@ -5362,7 +5602,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>9</v>
       </c>
@@ -5402,6 +5642,9 @@
       <c r="P82">
         <v>83104259139</v>
       </c>
+      <c r="Q82">
+        <v>0</v>
+      </c>
       <c r="R82">
         <v>4842</v>
       </c>
@@ -5409,7 +5652,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>9</v>
       </c>
@@ -5452,6 +5695,9 @@
       <c r="P83">
         <v>83129350013</v>
       </c>
+      <c r="Q83">
+        <v>0</v>
+      </c>
       <c r="R83">
         <v>3753</v>
       </c>
@@ -5459,7 +5705,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>9</v>
       </c>
@@ -5502,6 +5748,9 @@
       <c r="P84">
         <v>85956239318</v>
       </c>
+      <c r="Q84">
+        <v>0</v>
+      </c>
       <c r="R84">
         <v>5921</v>
       </c>
@@ -5509,7 +5758,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>9</v>
       </c>
@@ -5552,6 +5801,9 @@
       <c r="P85">
         <v>87717307011</v>
       </c>
+      <c r="Q85">
+        <v>0</v>
+      </c>
       <c r="R85">
         <v>453</v>
       </c>
@@ -5559,7 +5811,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>9</v>
       </c>
@@ -5599,6 +5851,9 @@
       <c r="P86" t="s">
         <v>38</v>
       </c>
+      <c r="Q86">
+        <v>0</v>
+      </c>
       <c r="R86">
         <v>112</v>
       </c>
@@ -5606,7 +5861,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>9</v>
       </c>
@@ -5649,6 +5904,9 @@
       <c r="P87">
         <v>87776741841</v>
       </c>
+      <c r="Q87">
+        <v>0</v>
+      </c>
       <c r="R87">
         <v>3571</v>
       </c>
@@ -5656,7 +5914,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>9</v>
       </c>
@@ -5699,6 +5957,9 @@
       <c r="P88">
         <v>87756118725</v>
       </c>
+      <c r="Q88">
+        <v>0</v>
+      </c>
       <c r="R88">
         <v>3654</v>
       </c>
@@ -5706,7 +5967,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>9</v>
       </c>
@@ -5749,6 +6010,9 @@
       <c r="P89">
         <v>85339327389</v>
       </c>
+      <c r="Q89">
+        <v>0</v>
+      </c>
       <c r="R89">
         <v>436</v>
       </c>
@@ -5756,7 +6020,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>9</v>
       </c>
@@ -5796,6 +6060,9 @@
       <c r="P90">
         <v>87849090207</v>
       </c>
+      <c r="Q90">
+        <v>0</v>
+      </c>
       <c r="R90">
         <v>5440</v>
       </c>
@@ -5803,7 +6070,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>9</v>
       </c>
@@ -5846,6 +6113,9 @@
       <c r="P91">
         <v>82144894140</v>
       </c>
+      <c r="Q91">
+        <v>0</v>
+      </c>
       <c r="R91">
         <v>7597</v>
       </c>
@@ -5853,7 +6123,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>9</v>
       </c>
@@ -5896,6 +6166,9 @@
       <c r="P92" t="s">
         <v>57</v>
       </c>
+      <c r="Q92">
+        <v>0</v>
+      </c>
       <c r="R92">
         <v>5479</v>
       </c>
@@ -5903,7 +6176,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>9</v>
       </c>
@@ -5946,6 +6219,9 @@
       <c r="P93">
         <v>85338308874</v>
       </c>
+      <c r="Q93">
+        <v>0</v>
+      </c>
       <c r="R93">
         <v>4754</v>
       </c>
@@ -5953,7 +6229,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>9</v>
       </c>
@@ -5996,6 +6272,9 @@
       <c r="P94">
         <v>82141027327</v>
       </c>
+      <c r="Q94">
+        <v>0</v>
+      </c>
       <c r="R94">
         <v>3491</v>
       </c>
@@ -6003,7 +6282,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>9</v>
       </c>
@@ -6046,6 +6325,9 @@
       <c r="P95">
         <v>85649367829</v>
       </c>
+      <c r="Q95">
+        <v>0</v>
+      </c>
       <c r="R95">
         <v>448</v>
       </c>
@@ -6053,7 +6335,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>9</v>
       </c>
@@ -6093,6 +6375,9 @@
       <c r="P96">
         <v>81338311765</v>
       </c>
+      <c r="Q96">
+        <v>0</v>
+      </c>
       <c r="R96">
         <v>12526</v>
       </c>
@@ -6100,7 +6385,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>9</v>
       </c>
@@ -6143,6 +6428,9 @@
       <c r="P97">
         <v>81615928815</v>
       </c>
+      <c r="Q97">
+        <v>0</v>
+      </c>
       <c r="R97">
         <v>762</v>
       </c>
@@ -6150,7 +6438,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>9</v>
       </c>
@@ -6190,6 +6478,9 @@
       <c r="P98">
         <v>89580229561</v>
       </c>
+      <c r="Q98">
+        <v>0</v>
+      </c>
       <c r="R98">
         <v>1632</v>
       </c>
@@ -6197,7 +6488,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>9</v>
       </c>
@@ -6237,6 +6528,9 @@
       <c r="P99">
         <v>89697451986</v>
       </c>
+      <c r="Q99">
+        <v>0</v>
+      </c>
       <c r="R99">
         <v>2725</v>
       </c>
@@ -6244,7 +6538,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>9</v>
       </c>
@@ -6287,6 +6581,9 @@
       <c r="P100" t="s">
         <v>57</v>
       </c>
+      <c r="Q100">
+        <v>0</v>
+      </c>
       <c r="R100">
         <v>2223</v>
       </c>
@@ -6294,7 +6591,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>9</v>
       </c>
@@ -6337,6 +6634,9 @@
       <c r="P101" t="s">
         <v>57</v>
       </c>
+      <c r="Q101">
+        <v>0</v>
+      </c>
       <c r="R101">
         <v>3636</v>
       </c>
@@ -6344,7 +6644,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>9</v>
       </c>
@@ -6387,6 +6687,9 @@
       <c r="P102" t="s">
         <v>57</v>
       </c>
+      <c r="Q102">
+        <v>0</v>
+      </c>
       <c r="R102">
         <v>119</v>
       </c>
@@ -6394,7 +6697,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>9</v>
       </c>
@@ -6437,6 +6740,9 @@
       <c r="P103" t="s">
         <v>57</v>
       </c>
+      <c r="Q103">
+        <v>0</v>
+      </c>
       <c r="R103">
         <v>45</v>
       </c>
@@ -6444,7 +6750,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>9</v>
       </c>
@@ -6487,6 +6793,9 @@
       <c r="P104" t="s">
         <v>57</v>
       </c>
+      <c r="Q104">
+        <v>0</v>
+      </c>
       <c r="R104">
         <v>813</v>
       </c>
@@ -6494,7 +6803,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>9</v>
       </c>
@@ -6537,6 +6846,9 @@
       <c r="P105" t="s">
         <v>57</v>
       </c>
+      <c r="Q105">
+        <v>0</v>
+      </c>
       <c r="R105">
         <v>6207</v>
       </c>
@@ -6544,7 +6856,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>9</v>
       </c>
@@ -6587,6 +6899,9 @@
       <c r="P106" t="s">
         <v>57</v>
       </c>
+      <c r="Q106">
+        <v>0</v>
+      </c>
       <c r="R106">
         <v>1329</v>
       </c>
@@ -6594,7 +6909,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>9</v>
       </c>
@@ -6637,6 +6952,9 @@
       <c r="P107" t="s">
         <v>57</v>
       </c>
+      <c r="Q107">
+        <v>0</v>
+      </c>
       <c r="R107">
         <v>21371</v>
       </c>
@@ -6644,7 +6962,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>9</v>
       </c>
@@ -6684,6 +7002,9 @@
       <c r="P108" t="s">
         <v>38</v>
       </c>
+      <c r="Q108">
+        <v>0</v>
+      </c>
       <c r="R108">
         <v>98</v>
       </c>
@@ -6691,7 +7012,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>9</v>
       </c>
@@ -6731,6 +7052,9 @@
       <c r="P109" t="s">
         <v>38</v>
       </c>
+      <c r="Q109">
+        <v>0</v>
+      </c>
       <c r="R109">
         <v>7325</v>
       </c>
@@ -6738,7 +7062,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>9</v>
       </c>
@@ -6781,6 +7105,9 @@
       <c r="P110" t="s">
         <v>57</v>
       </c>
+      <c r="Q110">
+        <v>0</v>
+      </c>
       <c r="R110">
         <v>3394</v>
       </c>
@@ -6788,7 +7115,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>9</v>
       </c>
@@ -6831,6 +7158,9 @@
       <c r="P111" t="s">
         <v>57</v>
       </c>
+      <c r="Q111">
+        <v>0</v>
+      </c>
       <c r="R111">
         <v>3152</v>
       </c>
@@ -6838,7 +7168,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>9</v>
       </c>
@@ -6881,6 +7211,9 @@
       <c r="P112" t="s">
         <v>57</v>
       </c>
+      <c r="Q112">
+        <v>0</v>
+      </c>
       <c r="R112">
         <v>7377</v>
       </c>
@@ -6888,7 +7221,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>9</v>
       </c>
@@ -6931,6 +7264,9 @@
       <c r="P113" t="s">
         <v>57</v>
       </c>
+      <c r="Q113">
+        <v>0</v>
+      </c>
       <c r="R113">
         <v>8571</v>
       </c>
@@ -6938,7 +7274,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>9</v>
       </c>
@@ -6981,6 +7317,9 @@
       <c r="P114" t="s">
         <v>57</v>
       </c>
+      <c r="Q114">
+        <v>0</v>
+      </c>
       <c r="R114">
         <v>2874</v>
       </c>
@@ -6988,7 +7327,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>9</v>
       </c>
@@ -7031,6 +7370,9 @@
       <c r="P115" t="s">
         <v>57</v>
       </c>
+      <c r="Q115">
+        <v>0</v>
+      </c>
       <c r="R115">
         <v>0</v>
       </c>
@@ -7038,7 +7380,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>9</v>
       </c>
@@ -7081,6 +7423,9 @@
       <c r="P116" t="s">
         <v>57</v>
       </c>
+      <c r="Q116">
+        <v>0</v>
+      </c>
       <c r="R116">
         <v>0</v>
       </c>
@@ -7088,7 +7433,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>9</v>
       </c>
@@ -7131,6 +7476,9 @@
       <c r="P117" t="s">
         <v>57</v>
       </c>
+      <c r="Q117">
+        <v>0</v>
+      </c>
       <c r="R117">
         <v>0</v>
       </c>
@@ -7138,7 +7486,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>9</v>
       </c>
@@ -7181,6 +7529,9 @@
       <c r="P118" t="s">
         <v>57</v>
       </c>
+      <c r="Q118">
+        <v>0</v>
+      </c>
       <c r="R118">
         <v>0</v>
       </c>
@@ -7188,7 +7539,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>9</v>
       </c>
@@ -7228,6 +7579,9 @@
       <c r="P119" t="s">
         <v>38</v>
       </c>
+      <c r="Q119">
+        <v>0</v>
+      </c>
       <c r="R119">
         <v>0</v>
       </c>
@@ -7235,7 +7589,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>9</v>
       </c>
@@ -7275,6 +7629,9 @@
       <c r="P120" t="s">
         <v>38</v>
       </c>
+      <c r="Q120">
+        <v>0</v>
+      </c>
       <c r="R120">
         <v>0</v>
       </c>
@@ -7282,7 +7639,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>9</v>
       </c>
@@ -7322,6 +7679,9 @@
       <c r="P121" t="s">
         <v>38</v>
       </c>
+      <c r="Q121">
+        <v>0</v>
+      </c>
       <c r="R121">
         <v>0</v>
       </c>
@@ -7329,7 +7689,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>9</v>
       </c>
@@ -7369,6 +7729,9 @@
       <c r="P122" t="s">
         <v>38</v>
       </c>
+      <c r="Q122">
+        <v>0</v>
+      </c>
       <c r="R122">
         <v>0</v>
       </c>
@@ -7376,7 +7739,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>9</v>
       </c>
@@ -7416,6 +7779,9 @@
       <c r="P123" t="s">
         <v>38</v>
       </c>
+      <c r="Q123">
+        <v>0</v>
+      </c>
       <c r="R123">
         <v>0</v>
       </c>
@@ -7423,7 +7789,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>9</v>
       </c>
@@ -7463,6 +7829,9 @@
       <c r="P124" t="s">
         <v>38</v>
       </c>
+      <c r="Q124">
+        <v>0</v>
+      </c>
       <c r="R124">
         <v>0</v>
       </c>
@@ -7470,7 +7839,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>9</v>
       </c>
@@ -7510,6 +7879,9 @@
       <c r="P125" t="s">
         <v>38</v>
       </c>
+      <c r="Q125">
+        <v>0</v>
+      </c>
       <c r="R125">
         <v>0</v>
       </c>
@@ -7517,7 +7889,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>9</v>
       </c>
@@ -7557,6 +7929,9 @@
       <c r="P126" t="s">
         <v>38</v>
       </c>
+      <c r="Q126">
+        <v>0</v>
+      </c>
       <c r="R126">
         <v>0</v>
       </c>
@@ -7564,7 +7939,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>9</v>
       </c>
@@ -7604,6 +7979,9 @@
       <c r="P127" t="s">
         <v>38</v>
       </c>
+      <c r="Q127">
+        <v>0</v>
+      </c>
       <c r="R127">
         <v>0</v>
       </c>
@@ -7611,7 +7989,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>9</v>
       </c>
@@ -7651,6 +8029,9 @@
       <c r="P128" t="s">
         <v>38</v>
       </c>
+      <c r="Q128">
+        <v>0</v>
+      </c>
       <c r="R128">
         <v>0</v>
       </c>
@@ -7658,7 +8039,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>9</v>
       </c>
@@ -7701,6 +8082,9 @@
       <c r="P129" t="s">
         <v>57</v>
       </c>
+      <c r="Q129">
+        <v>0</v>
+      </c>
       <c r="R129">
         <v>2416</v>
       </c>
@@ -7708,7 +8092,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>9</v>
       </c>
@@ -7751,6 +8135,9 @@
       <c r="P130" t="s">
         <v>57</v>
       </c>
+      <c r="Q130">
+        <v>0</v>
+      </c>
       <c r="R130">
         <v>3029</v>
       </c>
@@ -7758,7 +8145,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>9</v>
       </c>
@@ -7801,6 +8188,9 @@
       <c r="P131" t="s">
         <v>57</v>
       </c>
+      <c r="Q131">
+        <v>0</v>
+      </c>
       <c r="R131">
         <v>2609</v>
       </c>
@@ -7808,7 +8198,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>9</v>
       </c>
@@ -7851,6 +8241,9 @@
       <c r="P132" t="s">
         <v>57</v>
       </c>
+      <c r="Q132">
+        <v>0</v>
+      </c>
       <c r="R132">
         <v>1918</v>
       </c>
@@ -7858,7 +8251,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>9</v>
       </c>
@@ -7901,6 +8294,9 @@
       <c r="P133" t="s">
         <v>57</v>
       </c>
+      <c r="Q133">
+        <v>0</v>
+      </c>
       <c r="R133">
         <v>2047</v>
       </c>
@@ -7908,7 +8304,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>9</v>
       </c>
@@ -7951,6 +8347,9 @@
       <c r="P134" t="s">
         <v>57</v>
       </c>
+      <c r="Q134">
+        <v>0</v>
+      </c>
       <c r="R134">
         <v>4162</v>
       </c>
@@ -7958,7 +8357,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>9</v>
       </c>
@@ -8001,6 +8400,9 @@
       <c r="P135" t="s">
         <v>57</v>
       </c>
+      <c r="Q135">
+        <v>0</v>
+      </c>
       <c r="R135">
         <v>1866</v>
       </c>
@@ -8008,7 +8410,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>9</v>
       </c>
@@ -8051,6 +8453,9 @@
       <c r="P136" t="s">
         <v>57</v>
       </c>
+      <c r="Q136">
+        <v>0</v>
+      </c>
       <c r="R136">
         <v>972</v>
       </c>
@@ -8058,7 +8463,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>9</v>
       </c>
@@ -8101,6 +8506,9 @@
       <c r="P137" t="s">
         <v>57</v>
       </c>
+      <c r="Q137">
+        <v>0</v>
+      </c>
       <c r="R137">
         <v>1440</v>
       </c>
@@ -8108,7 +8516,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>9</v>
       </c>
@@ -8151,6 +8559,9 @@
       <c r="P138" t="s">
         <v>57</v>
       </c>
+      <c r="Q138">
+        <v>0</v>
+      </c>
       <c r="R138">
         <v>1560</v>
       </c>
@@ -8158,7 +8569,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>9</v>
       </c>
@@ -8201,6 +8612,9 @@
       <c r="P139" t="s">
         <v>57</v>
       </c>
+      <c r="Q139">
+        <v>0</v>
+      </c>
       <c r="R139">
         <v>1644</v>
       </c>
@@ -8208,7 +8622,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>9</v>
       </c>
@@ -8251,6 +8665,9 @@
       <c r="P140" t="s">
         <v>57</v>
       </c>
+      <c r="Q140">
+        <v>0</v>
+      </c>
       <c r="R140">
         <v>1699</v>
       </c>
@@ -8258,7 +8675,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>9</v>
       </c>
@@ -8301,6 +8718,9 @@
       <c r="P141" t="s">
         <v>57</v>
       </c>
+      <c r="Q141">
+        <v>0</v>
+      </c>
       <c r="R141">
         <v>1572</v>
       </c>
@@ -8308,7 +8728,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>9</v>
       </c>
@@ -8351,6 +8771,9 @@
       <c r="P142" t="s">
         <v>57</v>
       </c>
+      <c r="Q142">
+        <v>0</v>
+      </c>
       <c r="R142">
         <v>8801</v>
       </c>
@@ -8358,7 +8781,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>9</v>
       </c>
@@ -8401,6 +8824,9 @@
       <c r="P143" t="s">
         <v>57</v>
       </c>
+      <c r="Q143">
+        <v>0</v>
+      </c>
       <c r="R143">
         <v>1870</v>
       </c>
@@ -8408,7 +8834,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>9</v>
       </c>
@@ -8451,6 +8877,9 @@
       <c r="P144" t="s">
         <v>57</v>
       </c>
+      <c r="Q144">
+        <v>0</v>
+      </c>
       <c r="R144">
         <v>2845</v>
       </c>
@@ -8458,7 +8887,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>9</v>
       </c>
@@ -8501,6 +8930,9 @@
       <c r="P145" t="s">
         <v>57</v>
       </c>
+      <c r="Q145">
+        <v>0</v>
+      </c>
       <c r="R145">
         <v>2965</v>
       </c>
@@ -8508,7 +8940,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>9</v>
       </c>
@@ -8551,6 +8983,9 @@
       <c r="P146" t="s">
         <v>57</v>
       </c>
+      <c r="Q146">
+        <v>0</v>
+      </c>
       <c r="R146">
         <v>1875</v>
       </c>
@@ -8558,7 +8993,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>9</v>
       </c>
@@ -8601,6 +9036,9 @@
       <c r="P147" t="s">
         <v>57</v>
       </c>
+      <c r="Q147">
+        <v>0</v>
+      </c>
       <c r="R147">
         <v>1263</v>
       </c>
@@ -8608,7 +9046,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>9</v>
       </c>
@@ -8651,6 +9089,9 @@
       <c r="P148" t="s">
         <v>57</v>
       </c>
+      <c r="Q148">
+        <v>0</v>
+      </c>
       <c r="R148">
         <v>3198</v>
       </c>
@@ -8658,7 +9099,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>9</v>
       </c>
@@ -8701,6 +9142,9 @@
       <c r="P149" t="s">
         <v>57</v>
       </c>
+      <c r="Q149">
+        <v>0</v>
+      </c>
       <c r="R149">
         <v>1838</v>
       </c>
@@ -8708,7 +9152,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>9</v>
       </c>
@@ -8751,6 +9195,9 @@
       <c r="P150" t="s">
         <v>57</v>
       </c>
+      <c r="Q150">
+        <v>0</v>
+      </c>
       <c r="R150">
         <v>1636</v>
       </c>
@@ -8758,7 +9205,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>9</v>
       </c>
@@ -8801,6 +9248,9 @@
       <c r="P151" t="s">
         <v>57</v>
       </c>
+      <c r="Q151">
+        <v>0</v>
+      </c>
       <c r="R151">
         <v>2925</v>
       </c>
@@ -8808,7 +9258,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>9</v>
       </c>
@@ -8851,6 +9301,9 @@
       <c r="P152" t="s">
         <v>57</v>
       </c>
+      <c r="Q152">
+        <v>0</v>
+      </c>
       <c r="R152">
         <v>3426</v>
       </c>
@@ -8858,7 +9311,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>9</v>
       </c>
@@ -8901,6 +9354,9 @@
       <c r="P153" t="s">
         <v>57</v>
       </c>
+      <c r="Q153">
+        <v>0</v>
+      </c>
       <c r="R153">
         <v>1383</v>
       </c>
@@ -8908,7 +9364,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>9</v>
       </c>
@@ -8951,6 +9407,9 @@
       <c r="P154" t="s">
         <v>57</v>
       </c>
+      <c r="Q154">
+        <v>0</v>
+      </c>
       <c r="R154">
         <v>202</v>
       </c>
@@ -8958,7 +9417,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>9</v>
       </c>
@@ -9001,6 +9460,9 @@
       <c r="P155" t="s">
         <v>57</v>
       </c>
+      <c r="Q155">
+        <v>0</v>
+      </c>
       <c r="R155">
         <v>197</v>
       </c>
@@ -9008,7 +9470,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>9</v>
       </c>
@@ -9051,6 +9513,9 @@
       <c r="P156" t="s">
         <v>57</v>
       </c>
+      <c r="Q156">
+        <v>0</v>
+      </c>
       <c r="R156">
         <v>359</v>
       </c>
@@ -9058,7 +9523,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>9</v>
       </c>
@@ -9101,6 +9566,9 @@
       <c r="P157" t="s">
         <v>57</v>
       </c>
+      <c r="Q157">
+        <v>0</v>
+      </c>
       <c r="R157">
         <v>2012</v>
       </c>
@@ -9108,7 +9576,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>9</v>
       </c>
@@ -9151,6 +9619,9 @@
       <c r="P158" t="s">
         <v>57</v>
       </c>
+      <c r="Q158">
+        <v>0</v>
+      </c>
       <c r="R158">
         <v>2381</v>
       </c>
@@ -9158,7 +9629,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>9</v>
       </c>
@@ -9201,6 +9672,9 @@
       <c r="P159" t="s">
         <v>57</v>
       </c>
+      <c r="Q159">
+        <v>0</v>
+      </c>
       <c r="R159">
         <v>1479</v>
       </c>
@@ -9208,7 +9682,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>9</v>
       </c>
@@ -9251,6 +9725,9 @@
       <c r="P160" t="s">
         <v>57</v>
       </c>
+      <c r="Q160">
+        <v>0</v>
+      </c>
       <c r="R160">
         <v>668</v>
       </c>
@@ -9258,7 +9735,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="161" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>9</v>
       </c>
@@ -9301,6 +9778,9 @@
       <c r="P161" t="s">
         <v>57</v>
       </c>
+      <c r="Q161">
+        <v>0</v>
+      </c>
       <c r="R161">
         <v>3198</v>
       </c>
@@ -9308,7 +9788,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="162" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>9</v>
       </c>
@@ -9351,6 +9831,9 @@
       <c r="P162" t="s">
         <v>57</v>
       </c>
+      <c r="Q162">
+        <v>0</v>
+      </c>
       <c r="R162">
         <v>1231</v>
       </c>
@@ -9358,7 +9841,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="163" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>9</v>
       </c>
@@ -9401,6 +9884,9 @@
       <c r="P163" t="s">
         <v>57</v>
       </c>
+      <c r="Q163">
+        <v>0</v>
+      </c>
       <c r="R163">
         <v>2476</v>
       </c>
@@ -9408,7 +9894,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="164" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>9</v>
       </c>
@@ -9451,6 +9937,9 @@
       <c r="P164" t="s">
         <v>57</v>
       </c>
+      <c r="Q164">
+        <v>0</v>
+      </c>
       <c r="R164">
         <v>3437</v>
       </c>
@@ -9458,7 +9947,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="165" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>9</v>
       </c>
@@ -9501,6 +9990,9 @@
       <c r="P165" t="s">
         <v>57</v>
       </c>
+      <c r="Q165">
+        <v>0</v>
+      </c>
       <c r="R165">
         <v>2021</v>
       </c>
@@ -9508,7 +10000,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="166" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>9</v>
       </c>
@@ -9551,6 +10043,9 @@
       <c r="P166" t="s">
         <v>57</v>
       </c>
+      <c r="Q166">
+        <v>0</v>
+      </c>
       <c r="R166">
         <v>763</v>
       </c>
@@ -9558,7 +10053,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="167" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>9</v>
       </c>
@@ -9601,6 +10096,9 @@
       <c r="P167" t="s">
         <v>57</v>
       </c>
+      <c r="Q167">
+        <v>0</v>
+      </c>
       <c r="R167">
         <v>1458</v>
       </c>
@@ -9608,7 +10106,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="168" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>9</v>
       </c>
@@ -9651,6 +10149,9 @@
       <c r="P168" t="s">
         <v>57</v>
       </c>
+      <c r="Q168">
+        <v>0</v>
+      </c>
       <c r="R168">
         <v>1385</v>
       </c>
@@ -9658,7 +10159,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="169" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>9</v>
       </c>
@@ -9701,6 +10202,9 @@
       <c r="P169" t="s">
         <v>57</v>
       </c>
+      <c r="Q169">
+        <v>0</v>
+      </c>
       <c r="R169">
         <v>3349</v>
       </c>
@@ -9708,7 +10212,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="170" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>9</v>
       </c>
@@ -9751,6 +10255,9 @@
       <c r="P170" t="s">
         <v>57</v>
       </c>
+      <c r="Q170">
+        <v>0</v>
+      </c>
       <c r="R170">
         <v>1288</v>
       </c>
@@ -9758,7 +10265,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="171" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>9</v>
       </c>
@@ -9801,6 +10308,9 @@
       <c r="P171" t="s">
         <v>57</v>
       </c>
+      <c r="Q171">
+        <v>0</v>
+      </c>
       <c r="R171">
         <v>3511</v>
       </c>
@@ -9808,7 +10318,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="172" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>9</v>
       </c>
@@ -9851,6 +10361,9 @@
       <c r="P172" t="s">
         <v>57</v>
       </c>
+      <c r="Q172">
+        <v>0</v>
+      </c>
       <c r="R172">
         <v>806</v>
       </c>
@@ -9858,7 +10371,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="173" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>9</v>
       </c>
@@ -9901,6 +10414,9 @@
       <c r="P173" t="s">
         <v>57</v>
       </c>
+      <c r="Q173">
+        <v>0</v>
+      </c>
       <c r="R173">
         <v>1166</v>
       </c>
@@ -9908,7 +10424,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="174" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>9</v>
       </c>
@@ -9950,6 +10466,9 @@
       </c>
       <c r="P174" t="s">
         <v>57</v>
+      </c>
+      <c r="Q174">
+        <v>0</v>
       </c>
       <c r="R174">
         <v>1644</v>

</xml_diff>